<commit_message>
actualizacion de la solucion
</commit_message>
<xml_diff>
--- a/ganadoras_premio_nobel.xlsx
+++ b/ganadoras_premio_nobel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Motivación</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha_Scraping</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +491,11 @@
           <t>«En reconocimiento a los extraordinarios servicios que han prestado con sus investigaciones conjuntas sobre los fenómenos de la radiación descubierta junto al profesor Henri Becquerel».[9]​</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -513,6 +523,11 @@
           <t>Presidenta honoraria de laOficina Internacional por la Paz,Berna,Suiza. Autora deLay Down Your Arms.[11]​</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -540,6 +555,11 @@
           <t>«En reconocimiento al elevado idealismo, la vívida imaginación y la percepción espiritual que caracterizan sus escritos».[12]​</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,6 +587,11 @@
           <t>Por su descubrimiento delradioy elpolonio.[13]​</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -594,6 +619,11 @@
           <t>«Por sus escritos inspiradamente idealistas, que con claridad plástica dibujan la vida en su isla natal y que con profundidad y simpatía tratan los problemas humanos en general».[14]​</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -621,6 +651,11 @@
           <t>«Principalmente por sus poderosas descripciones de la vida de los nórdicos durante la Edad Media».[15]​</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +683,11 @@
           <t>Socióloga, pionera del trabajo social y el feminismo, presidenta de laLiga Internacional de Mujeres por la Paz y la Libertad.[16]​[17]​</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -675,6 +715,11 @@
           <t>«Por su síntesis de nuevos elementos radiactivos».[18]​</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -702,6 +747,11 @@
           <t>«Por sus descripciones ricas y verdaderamente épicas de la vida campesina en China y por sus obras maestras biográficas».[19]​</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -729,6 +779,11 @@
           <t>«Por su poesía lírica que, inspirada por poderosas emociones, ha hecho de su nombre un símbolo de las aspiraciones idealistas de todo el mundo latinoamericano».[20]​</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -756,6 +811,11 @@
           <t>Anteriormente profesora de Historia y Sociología, presidenta honoraria de la Liga Internacional de Mujeres por la Paz y la Libertad.[21]​</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -783,6 +843,11 @@
           <t>«Por su descubrimiento del proceso de la conversión catalítica delglucógeno».[22]​</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -810,6 +875,11 @@
           <t>«Por sus descubrimientos sobre laestructura de capas nuclear».[23]​</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -837,6 +907,11 @@
           <t>«Por determinar las estructuras de importantes sustancias bioquímicas por medio detécnicas de rayos X».[24]​</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -864,6 +939,11 @@
           <t>«Por su destacada escritura lírica y dramática, que interpreta el destino de Israel con fuerza conmovedora».[25]​</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -891,6 +971,11 @@
           <t>Fundadoras del Northern Ireland Peace Movement (Movimiento por la Paz de Irlanda del Norte), después renombrado Community of Peace People (Comunidad de Gente Pacífica).[26]​</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -918,6 +1003,11 @@
           <t>«Por el desarrollo delradioinmunoanálisisde lashormonas peptídicas».[27]​</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -945,6 +1035,11 @@
           <t>Líder de lasMisioneras de la Caridad,Calcuta.[28]​</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -972,6 +1067,11 @@
           <t>Exministra del gabinete, diplomática y escritora.[29]​</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -999,6 +1099,11 @@
           <t>«Por su descubrimiento de loselementos genéticos móviles».[30]​</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1026,6 +1131,11 @@
           <t>«Por su descubrimiento de losfactores de crecimiento».[31]​</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1053,6 +1163,11 @@
           <t>«Por su descubrimiento de importantes principios en eltratamiento con fármacos».[32]​</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1080,6 +1195,11 @@
           <t>«Quien a través de su magnífica escritura épica —en palabras de Alfred Nobel— ha sido de gran beneficio para la humanidad».[33]​</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1107,6 +1227,11 @@
           <t>«Por su lucha no violenta por la democracia y los derechos humanos».[34]​</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1134,6 +1259,11 @@
           <t>«En reconocimiento a su trabajo por la justicia social y la reconciliación etno-cultural basada en el respeto de los derechos de los pueblos indígenas».[35]​</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1161,6 +1291,11 @@
           <t>«Quien en novelas caracterizadas por su fuerza visionaria y transcendencia poética, da vida a un aspecto esencial de la realidad estadounidense».[36]​</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1188,6 +1323,11 @@
           <t>«Por sus descubrimientos sobre el control genético deldesarrollo embrionariotemprano».[37]​</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1215,6 +1355,11 @@
           <t>«Por la poesía que con precisión irónica permite al contexto histórico y biológico salir a la luz en fragmentos de la realidad humana».[38]​</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1242,6 +1387,11 @@
           <t>«Por su trabajo para la prohibición y limpieza de minas antipersonales».[39]​</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1269,6 +1419,11 @@
           <t>«Por sus esfuerzos por la democracia y los derechos humanos. Se ha centrado especialmente en la lucha por los derechos de las mujeres y los niños».[40]​</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1296,6 +1451,11 @@
           <t>«Por su flujo musical de voces y contravoces en novelas y obras teatrales que con extraordinario celo lingüístico revelan lo absurdo de los clichés de la sociedad y su poder subyugante».[41]​</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1323,6 +1483,11 @@
           <t>«Por su contribución al desarrollo sustentable, la democracia y la paz».[42]​</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1350,6 +1515,11 @@
           <t>«Por su descubrimiento de losreceptores olfatoriosy la organización delsistema olfativo».[43]​</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1377,6 +1547,11 @@
           <t>«La narradora épica de la experiencia femenina, quien con escepticismo, ardor y poder visionario ha sometido a una civilización dividida al escrutinio».[44]​</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1404,6 +1579,11 @@
           <t>«Por su descubrimiento delvirus de la inmunodeficiencia humana».[45]​</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1431,6 +1611,11 @@
           <t>«Por el descubrimiento de cómo los cromosomas son protegidos por los telómeros y la enzima telomerasa».[46]​</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1458,6 +1643,11 @@
           <t>«Por el estudio de la estructura y función de los ribosomas».[47]​</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1485,6 +1675,11 @@
           <t>«Quien, con la concentración de la poesía y la franqueza de la prosa, describe el paisaje de los desposeídos».[48]​</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1512,6 +1707,11 @@
           <t>«Por su análisis de la gobernanza económica, especialmente los bienes comunes».[49]​</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1539,6 +1739,11 @@
           <t>«Por su lucha sin violencia por la seguridad de las mujeres y el derecho de la mujer a participar plenamente en la labor de consolidación de la paz».[50]​</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1566,6 +1771,11 @@
           <t>«Maestra del cuento contemporáneo».[51]​</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1593,6 +1803,11 @@
           <t>«Por sus descubrimientos de células que constituyen un sistema de posicionamiento en el cerebro».[52]​</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1620,6 +1835,11 @@
           <t>«Por su lucha contra la represión de los niños y jóvenes, y por el derecho de todos los niños a la educación».[53]​</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1647,6 +1867,11 @@
           <t>«Por sus descubrimientos de una nueva terapia contra lamalaria».[54]​</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1674,6 +1899,11 @@
           <t>«Por sus escritos polifónicos, un monumento al sufrimiento y valor en nuestro tiempo».[55]​</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1701,6 +1931,11 @@
           <t>«Por su método para generar pulsos ópticos ultra cortos de alta intensidad».[56]​</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1728,6 +1963,11 @@
           <t>«Por la evolución dirigida de enzimas».[57]​</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1755,6 +1995,11 @@
           <t>«Por sus esfuerzos para acabar con el uso de la violencia sexual como arma en guerras y conflictos armados»[58]​</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1782,6 +2027,11 @@
           <t>«Por su imaginación narrativa que con pasión enciclopédica representa el cruce de fronteras como una forma de vida».[59]​</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1809,6 +2059,11 @@
           <t>«Por su enfoque experimental para aliviar la pobreza global».[60]​</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1836,6 +2091,11 @@
           <t>«Por el descubrimiento de un objeto compacto supermasivo en el centro de nuestra galaxia».[61]​</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1863,6 +2123,11 @@
           <t>«Por el desarrollo de un método para la edición del genoma».[62]​</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1890,6 +2155,11 @@
           <t>«Por su inconfundible voz poética que con austera belleza hace universal la existencia individual».[63]​</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1917,6 +2187,11 @@
           <t>«Por sus esfuerzos para salvaguardar la libertad de expresión, como condición para la democracia y la paz duradera».[64]​</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1944,6 +2219,11 @@
           <t>«Por el desarrollo de laquímica clicky laquímica bioortogonal».[65]​</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1971,6 +2251,11 @@
           <t>«Por el coraje y la agudeza clínica con la que descubre las raíces, los extrañamientos y las restricciones colectivas de la memoria personal».[66]​</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1998,6 +2283,11 @@
           <t>«Por avanzar nuestra comprensión de los resultados del trabajo de las mujeres».[67]​</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2025,6 +2315,11 @@
           <t>«Por su lucha contra la opresión de las mujeres en Irán y su lucha por promover los derechos humanos para todos»[68]​</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2052,6 +2347,11 @@
           <t>«Por sus métodos experimentales que generan pulsos de luz deattosegundospara el estudio de la dinámica de los electrones en la materia»[69]​</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2079,6 +2379,11 @@
           <t>«Por sus descubrimientos sobre modificaciones de bases de nucleósidos que permitieron el desarrollo devacunasefectivas de ARNm contra elCOVID-19»[70]​</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2104,6 +2409,11 @@
       <c r="E62" t="inlineStr">
         <is>
           <t>«Por su intensa prosa poética que confronta traumas históricos y expone la fragilidad de la vida humana».[71]​</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2025-05-11 19:22:43</t>
         </is>
       </c>
     </row>

</xml_diff>